<commit_message>
ADDED: .csv file (changed the default save directory); updated some default values and resulting files
</commit_message>
<xml_diff>
--- a/benchmark_data.xlsx
+++ b/benchmark_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2e60\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{968E09BC-A688-4CAC-B45F-BCBD37BD9716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4333F8D8-8D16-418B-9CE2-3844AAFEC60F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -596,24 +596,27 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1020,10 +1023,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H44"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H38" activeCellId="9" sqref="H39:H43 H32:H36 H26:H30 H20:H24 H17:H18 H15 H8:H12 H2:H6 H14 H38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15"/>
@@ -1037,1133 +1043,1123 @@
     <col min="8" max="8" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="10" customFormat="1" ht="15.75">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:8" s="7" customFormat="1" ht="15.75">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>1179</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>690</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>64.895499999999998</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>265.471</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>4</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>1179</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>816</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>65.362799999999993</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>71.014399999999995</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>4</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>1179</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>765</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>66.992199999999997</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>73.732200000000006</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>4</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>1179</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>575</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>48.886400000000002</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>219.017</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>4</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>1179</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>927</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>47.0336</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>119.633</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>4</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="5" customFormat="1">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:8" s="2" customFormat="1">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="4" t="s">
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2">
-        <v>65</v>
-      </c>
-      <c r="D8" s="2">
-        <v>49</v>
-      </c>
-      <c r="E8" s="2">
-        <v>48.717100000000002</v>
-      </c>
-      <c r="F8" s="2">
-        <v>239.31700000000001</v>
-      </c>
-      <c r="G8" s="2">
+      <c r="C8" s="1">
+        <v>262</v>
+      </c>
+      <c r="D8" s="1">
+        <v>177</v>
+      </c>
+      <c r="E8" s="8">
+        <v>85.350099999999998</v>
+      </c>
+      <c r="F8" s="9">
+        <v>260.71300000000002</v>
+      </c>
+      <c r="G8" s="1">
         <v>10</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2">
-        <v>65</v>
-      </c>
-      <c r="D9" s="2">
-        <v>55</v>
-      </c>
-      <c r="E9" s="2">
-        <v>46.506</v>
-      </c>
-      <c r="F9" s="2">
-        <v>47.484200000000001</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="C9" s="1">
+        <v>262</v>
+      </c>
+      <c r="D9" s="1">
+        <v>193</v>
+      </c>
+      <c r="E9" s="1">
+        <v>82.859300000000005</v>
+      </c>
+      <c r="F9" s="9">
+        <v>84.059100000000001</v>
+      </c>
+      <c r="G9" s="1">
         <v>10</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="2">
-        <v>65</v>
-      </c>
-      <c r="D10" s="2">
-        <v>55</v>
-      </c>
-      <c r="E10" s="2">
-        <v>48.346299999999999</v>
-      </c>
-      <c r="F10" s="2">
-        <v>52.900100000000002</v>
-      </c>
-      <c r="G10" s="2">
+      <c r="C10" s="1">
+        <v>262</v>
+      </c>
+      <c r="D10" s="1">
+        <v>180</v>
+      </c>
+      <c r="E10" s="1">
+        <v>82.927199999999999</v>
+      </c>
+      <c r="F10" s="1">
+        <v>87.617000000000004</v>
+      </c>
+      <c r="G10" s="1">
         <v>10</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2">
-        <v>65</v>
-      </c>
-      <c r="D11" s="2">
-        <v>50</v>
-      </c>
-      <c r="E11" s="2">
-        <v>46.4176</v>
-      </c>
-      <c r="F11" s="2">
-        <v>206.435</v>
-      </c>
-      <c r="G11" s="2">
+      <c r="C11" s="1">
+        <v>262</v>
+      </c>
+      <c r="D11" s="1">
+        <v>169</v>
+      </c>
+      <c r="E11" s="1">
+        <v>80.543300000000002</v>
+      </c>
+      <c r="F11" s="1">
+        <v>236.916</v>
+      </c>
+      <c r="G11" s="1">
         <v>10</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="2">
-        <v>65</v>
-      </c>
-      <c r="D12" s="2">
-        <v>55</v>
-      </c>
-      <c r="E12" s="2">
-        <v>45.191899999999997</v>
-      </c>
-      <c r="F12" s="2">
-        <v>113.852</v>
-      </c>
-      <c r="G12" s="2">
+      <c r="C12" s="1">
+        <v>262</v>
+      </c>
+      <c r="D12" s="1">
+        <v>194</v>
+      </c>
+      <c r="E12" s="1">
+        <v>82.3476</v>
+      </c>
+      <c r="F12" s="1">
+        <v>152.21899999999999</v>
+      </c>
+      <c r="G12" s="1">
         <v>10</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:8" s="2" customFormat="1">
+      <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="4" t="s">
+      <c r="C13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>1386</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>536</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>548.53899999999999</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>645.32100000000003</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <v>5.0323500000000001</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="1">
         <v>5.9674899999999997</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>1386</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>597</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>541.51599999999996</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>545.34500000000003</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <v>5.0323500000000001</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="1">
         <v>5.9674899999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="8" customFormat="1">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:8" s="4" customFormat="1">
+      <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="7" t="s">
+      <c r="C16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>1386</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>500</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>462.90899999999999</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>628.79100000000005</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="1">
         <v>5.0323500000000001</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="1">
         <v>5.9674899999999997</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>1386</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>800</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>458.31</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>823.13300000000004</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="1">
         <v>5.0323500000000001</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="1">
         <v>5.9674899999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="5" customFormat="1">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:8" s="2" customFormat="1">
+      <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="4" t="s">
+      <c r="C19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>1491</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>776</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>5.2306400000000002</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>102.259</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="1">
         <v>7</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>1491</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>883</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="1">
         <v>5.33331</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>8.4458000000000002</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="1">
         <v>7</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>1491</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>859</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="1">
         <v>5.7712599999999998</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <v>12.644600000000001</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="1">
         <v>7</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>1491</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>657</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="1">
         <v>6.0541200000000002</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="1">
         <v>172.32300000000001</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="1">
         <v>7</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>17</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>1491</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>1046</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="1">
         <v>6.39703</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>82.167900000000003</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="1">
         <v>7</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="5" customFormat="1">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:8" s="2" customFormat="1">
+      <c r="A25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H25" s="4" t="s">
+      <c r="C25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>2762</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="1">
         <v>1298</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="1">
         <v>312.73099999999999</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="1">
         <v>416.52600000000001</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="1">
         <v>21.9422</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="1">
         <v>14.607900000000001</v>
       </c>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>2762</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <v>1344</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="1">
         <v>314.221</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="1">
         <v>319.02699999999999</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="1">
         <v>21.9422</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="1">
         <v>14.607900000000001</v>
       </c>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>11</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>2762</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>913</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="1">
         <v>314.80799999999999</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="1">
         <v>341.64600000000002</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="1">
         <v>21.9422</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="1">
         <v>14.607900000000001</v>
       </c>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>12</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>2762</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <v>1090</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="1">
         <v>313.64699999999999</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="1">
         <v>484.28</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="1">
         <v>21.9422</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="1">
         <v>14.607900000000001</v>
       </c>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>2762</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="1">
         <v>1646</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="1">
         <v>368.20299999999997</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="1">
         <v>480.351</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="1">
         <v>21.9422</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="1">
         <v>14.607900000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:8" s="5" customFormat="1">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:8" s="2" customFormat="1">
+      <c r="A31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H31" s="4" t="s">
+      <c r="C31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <v>1161</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="1">
         <v>649</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="1">
         <v>122.68600000000001</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="1">
         <v>309.77800000000002</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="1">
         <v>56.0578</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="1">
         <v>25.245999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <v>1161</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="1">
         <v>450</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="1">
         <v>39.393099999999997</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="1">
         <v>41.738700000000001</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33" s="1">
         <v>56.0578</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33" s="1">
         <v>25.245999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="1">
         <v>1161</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="1">
         <v>515</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="1">
         <v>39.034500000000001</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="1">
         <v>65.431600000000003</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34" s="1">
         <v>56.0578</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="1">
         <v>25.245999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="1">
         <v>1161</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="1">
         <v>349</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="1">
         <v>39.267299999999999</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="1">
         <v>202.495</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35" s="1">
         <v>56.0578</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35" s="1">
         <v>25.245999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="1">
         <v>1161</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="1">
         <v>763</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="1">
         <v>39.863</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F36" s="1">
         <v>179.67599999999999</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36" s="1">
         <v>56.0578</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36" s="1">
         <v>25.245999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:8" s="5" customFormat="1">
-      <c r="A37" s="3" t="s">
+    <row r="37" spans="1:8" s="2" customFormat="1">
+      <c r="A37" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H37" s="4" t="s">
+      <c r="C37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="1" t="s">
+      <c r="A38" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="1">
         <v>1670</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="1">
         <v>1110</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="1">
         <v>250.70099999999999</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F38" s="1">
         <v>442.714</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G38" s="1">
         <v>7.6934199999999997</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H38" s="1">
         <v>3.5417800000000002</v>
       </c>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="1" t="s">
+      <c r="A39" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="1">
         <v>1670</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="1">
         <v>1087</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="1">
         <v>244.904</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F39" s="1">
         <v>249.32400000000001</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G39" s="1">
         <v>7.6934199999999997</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H39" s="1">
         <v>3.5417800000000002</v>
       </c>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="1" t="s">
+      <c r="A40" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="1">
         <v>1670</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="1">
         <v>922</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="1">
         <v>242.62799999999999</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40" s="1">
         <v>260.71199999999999</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40" s="1">
         <v>7.6934199999999997</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H40" s="1">
         <v>3.5417800000000002</v>
       </c>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="1">
         <v>1670</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="1">
         <v>966</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="1">
         <v>243.40600000000001</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="1">
         <v>413.822</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41" s="1">
         <v>7.6934199999999997</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41" s="1">
         <v>3.5417800000000002</v>
       </c>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="1" t="s">
+      <c r="A42" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="1">
         <v>1670</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="1">
         <v>1270</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="1">
         <v>239.94300000000001</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42" s="1">
         <v>337.78</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="1">
         <v>7.6934199999999997</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="1">
         <v>3.5417800000000002</v>
       </c>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="1" t="s">
+      <c r="A43" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="1">
         <v>1670</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="1">
         <v>1172</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43" s="1">
         <v>241.71700000000001</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F43" s="1">
         <v>442.23099999999999</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G43" s="1">
         <v>7.6934199999999997</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="1">
         <v>3.5417800000000002</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F43">
@@ -2191,6 +2187,8 @@
       <formula>MAX($H:$H)</formula>
     </cfRule>
   </conditionalFormatting>
+  <printOptions headings="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
 </worksheet>
 </file>
</xml_diff>